<commit_message>
Metodos create y delete
</commit_message>
<xml_diff>
--- a/Eventos.xlsx
+++ b/Eventos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b09aa766bde0394/Documentos/tutorials/adminlte/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Proyectos\adminlte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{B2D11F12-2C67-46E5-9139-C6D618193978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87C62EA5-9E59-42FE-90C4-70D4705FDDA3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDEC030-53EA-424A-8698-DDC118D73E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{67C8542A-56DE-402D-B336-4E659CBDF565}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67C8542A-56DE-402D-B336-4E659CBDF565}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Primer Evento</t>
   </si>
   <si>
-    <t>Reunión</t>
-  </si>
-  <si>
     <t>Segundo Evento</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Tipo</t>
+  </si>
+  <si>
+    <t>Por defecto</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +439,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -453,12 +453,12 @@
         <v>45008.833333333336</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>45010.583333333336</v>
@@ -467,12 +467,12 @@
         <v>45010.625</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>45011.416666666664</v>
@@ -481,7 +481,7 @@
         <v>45011.541666666664</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Colores tipos de eventos
</commit_message>
<xml_diff>
--- a/Eventos.xlsx
+++ b/Eventos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Proyectos\adminlte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b09aa766bde0394/Documentos/tutorials/adminlte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDEC030-53EA-424A-8698-DDC118D73E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BDDEC030-53EA-424A-8698-DDC118D73E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{035A2530-D07C-4D2D-968F-EC74FB3DBEA2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67C8542A-56DE-402D-B336-4E659CBDF565}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{67C8542A-56DE-402D-B336-4E659CBDF565}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Título</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Por defecto</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>Reunion</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +473,7 @@
         <v>45010.625</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -481,7 +487,7 @@
         <v>45011.541666666664</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>